<commit_message>
Added the ability to dynamically update the punch inner and outer section as the punch moves into the die
</commit_message>
<xml_diff>
--- a/sandbox/pellet_sintering/version-descriptor.xlsx
+++ b/sandbox/pellet_sintering/version-descriptor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Input-files" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -31,10 +31,25 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
+    <t xml:space="preserve">pellet_v5_20180527.i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the punch’s outer boundary was split to allow for dirichlet temperature boundary condition to be applied to upper part and thermal contact condition to be applied on the lower part which is inside the die.</t>
+  </si>
+  <si>
     <t xml:space="preserve">pellet_v6_20180612.i</t>
   </si>
   <si>
     <t xml:space="preserve">temperature boundary condition uses a composite function to allow temperature gradient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pellet_v7_20180706.i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pellet_v4_20180517.e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pellet_v5_20180529.e</t>
   </si>
 </sst>
 </file>
@@ -49,6 +64,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -70,6 +86,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,16 +157,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -160,12 +177,25 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -184,15 +214,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -203,10 +234,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -227,7 +271,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -241,7 +285,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -262,12 +306,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
added files for simulating punch motion
</commit_message>
<xml_diff>
--- a/sandbox/pellet_sintering/version-descriptor.xlsx
+++ b/sandbox/pellet_sintering/version-descriptor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Input-files" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -44,6 +44,15 @@
   </si>
   <si>
     <t xml:space="preserve">pellet_v7_20180706.i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">penalty based boundary condition implemented. It allows to turn on &amp; off temp bc based on spatial location.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pellet_v8_20180612.i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">punch motion implemented</t>
   </si>
   <si>
     <t xml:space="preserve">pellet_v4_20180517.e</t>
@@ -157,10 +166,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -197,6 +206,17 @@
       <c r="A7" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="B7" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -216,7 +236,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -236,12 +256,12 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>3</v>

</xml_diff>